<commit_message>
Nomenclatura adecauda Encuesta Satisfaccion Cinovatec Mayo
</commit_message>
<xml_diff>
--- a/qualtcom/Procesos/Encuestas de Satisfaccion/Cinovatec_EncuestaSatisfaccion-150527.xlsx
+++ b/qualtcom/Procesos/Encuestas de Satisfaccion/Cinovatec_EncuestaSatisfaccion-150527.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\proyecto\qualtcom\Procesos\Encuestas de Satisfaccion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\qtp\qualtcom\Procesos\Encuestas de Satisfaccion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="69">
   <si>
     <t>Encuesta de Satisfacción al Cliente</t>
   </si>
@@ -245,6 +245,9 @@
   </si>
   <si>
     <t>SE notifica que la explicacion de la solucion ya es mas comprensible y no tan cerrada.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
@@ -1444,7 +1447,7 @@
   <dimension ref="A1:AMK22"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1511,6 +1514,9 @@
       <c r="D6" s="125"/>
       <c r="E6" s="125"/>
       <c r="F6" s="125"/>
+      <c r="G6" s="1" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="7" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B7" s="68" t="s">

</xml_diff>

<commit_message>
Encuesta de satisfaccion cinovatec Mayo, actualizado por error en escritura de persona entrevistada
</commit_message>
<xml_diff>
--- a/qualtcom/Procesos/Encuestas de Satisfaccion/Cinovatec_EncuestaSatisfaccion-150527.xlsx
+++ b/qualtcom/Procesos/Encuestas de Satisfaccion/Cinovatec_EncuestaSatisfaccion-150527.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\qtp\qualtcom\Procesos\Encuestas de Satisfaccion\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zepeda\Documents\qtp\qualtcom\Procesos\Encuestas de Satisfaccion\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="817"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="817" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Inf. Gral." sheetId="1" r:id="rId1"/>
@@ -232,9 +232,6 @@
     <t>Describir aquí las cosas que el cliente comenta acerca de la pregunta que se acaba de realizar. Escribir textualmente los comentarios del entrevistado buscando quedar claro en lo que desea expresar</t>
   </si>
   <si>
-    <t>Mariano Soto</t>
-  </si>
-  <si>
     <t>Mayra Tejeda</t>
   </si>
   <si>
@@ -248,6 +245,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Adriana Lira Beltran</t>
   </si>
 </sst>
 </file>
@@ -1446,7 +1446,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AMK22"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView showGridLines="0" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -1498,7 +1498,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="125" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="D5" s="125"/>
       <c r="E5" s="125"/>
@@ -1509,13 +1509,13 @@
         <v>3</v>
       </c>
       <c r="C6" s="125" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="D6" s="125"/>
       <c r="E6" s="125"/>
       <c r="F6" s="125"/>
       <c r="G6" s="1" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="7" spans="1:13" ht="13.9" customHeight="1" x14ac:dyDescent="0.2">
@@ -1534,7 +1534,7 @@
         <v>5</v>
       </c>
       <c r="C8" s="125" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D8" s="125"/>
       <c r="E8" s="125"/>
@@ -1682,8 +1682,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:BT99"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C4" sqref="C4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1798,7 +1798,7 @@
       <c r="A4" s="103"/>
       <c r="B4" s="103"/>
       <c r="C4" s="92" t="s">
-        <v>63</v>
+        <v>68</v>
       </c>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
@@ -1873,7 +1873,7 @@
       <c r="A5" s="104"/>
       <c r="B5" s="104"/>
       <c r="C5" s="93" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="D5" s="17"/>
       <c r="E5" s="17"/>
@@ -2487,7 +2487,7 @@
         <v>4</v>
       </c>
       <c r="E13" s="100" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="F13" s="103"/>
       <c r="G13" s="119"/>

</xml_diff>